<commit_message>
Added estimated cleaning coasts
</commit_message>
<xml_diff>
--- a/Open Source Autonomous Model_forgithub_3.29.19_v4.xlsx
+++ b/Open Source Autonomous Model_forgithub_3.29.19_v4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiakeeney/Desktop/Autonomous Vehicles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ARK-Invest-Autonomous-Taxi-Price-Per-Mile-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144EDF34-05A1-4E9F-9875-1A3E3A8143D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="460" windowWidth="32240" windowHeight="18060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARK Disclosure " sheetId="4" r:id="rId1"/>
@@ -21,7 +22,7 @@
   <definedNames>
     <definedName name="Penetration">OFFSET([1]S_Curve!$B$11,0,0,COUNTA([1]S_Curve!$B$11:$B$110),1)</definedName>
     <definedName name="Saturation">OFFSET([1]S_Curve!$C$11,0,0,COUNTA([1]S_Curve!$C$11:$C$110),1)</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Price Per Mi Model'!$C$27</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Price Per Mi Model'!$C$28</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
@@ -34,7 +35,7 @@
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Price Per Mi Model'!$C$65</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Price Per Mi Model'!$C$67</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
@@ -49,10 +50,16 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
     <definedName name="Year">OFFSET([1]S_Curve!$A$11,0,0,COUNTA([1]S_Curve!$A$11:$A$110),1)</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>Key:</t>
   </si>
@@ -352,18 +359,27 @@
   <si>
     <t>Each autonomous car can accomodate 8.6 people @ 13,500 miles per year per car / 219,000 total possible autonomous miles possible per car per year (asuming 25MPH x 24 hrs/day x 365 days/year). Formula subject to updates.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Cleaning </t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>65USD Cleaning / Week (Exterior &amp; Interial manual cleaning price in SF)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -570,7 +586,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +639,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -771,13 +793,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
@@ -800,7 +822,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -862,7 +884,7 @@
     </xf>
     <xf numFmtId="3" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -872,7 +894,7 @@
     <xf numFmtId="1" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,7 +902,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -890,7 +912,7 @@
     <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="38" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -915,7 +937,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -924,8 +946,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="4" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="28" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -945,38 +967,50 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Bold" xfId="5"/>
-    <cellStyle name="Comma 2" xfId="4"/>
-    <cellStyle name="Comma 2 2" xfId="6"/>
-    <cellStyle name="Comma 2 3" xfId="7"/>
-    <cellStyle name="Comma 3" xfId="3"/>
-    <cellStyle name="Comma 4" xfId="8"/>
-    <cellStyle name="Currency 2" xfId="9"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="10"/>
-    <cellStyle name="Normal 2 2" xfId="11"/>
-    <cellStyle name="Normal 3" xfId="12"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="13"/>
-    <cellStyle name="Percent 2 2" xfId="14"/>
-    <cellStyle name="Percent 2 3" xfId="15"/>
-    <cellStyle name="Percent 3" xfId="2"/>
-    <cellStyle name="Percent 4" xfId="16"/>
-    <cellStyle name="Title-2" xfId="17"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Bold" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 4" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Currency 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Link" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="28" builtinId="8"/>
+    <cellStyle name="Normal 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Percent 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Percent 2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 2 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Percent 3" xfId="2" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Percent 4" xfId="16" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Title-2" xfId="17" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1017,7 +1051,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAAFB6BF-00C5-484E-912C-F879ACBF6F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAAFB6BF-00C5-484E-912C-F879ACBF6F70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1062,7 +1096,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01437F55-F667-724E-B448-6EEB2DCFC319}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01437F55-F667-724E-B448-6EEB2DCFC319}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1101,354 +1135,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="S_Curve (2)"/>
       <sheetName val="S_Curve"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="11">
-          <cell r="A11">
-            <v>2011</v>
-          </cell>
-          <cell r="B11">
-            <v>0.12328767123287669</v>
-          </cell>
-          <cell r="C11">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>2012</v>
-          </cell>
-          <cell r="B12">
-            <v>0.17770393402630352</v>
-          </cell>
-          <cell r="C12">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>2013</v>
-          </cell>
-          <cell r="B13">
-            <v>0.25606981809120444</v>
-          </cell>
-          <cell r="C13">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>2014</v>
-          </cell>
-          <cell r="B14">
-            <v>0.36885245901639319</v>
-          </cell>
-          <cell r="C14">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>2015</v>
-          </cell>
-          <cell r="B15">
-            <v>0.53101483706617747</v>
-          </cell>
-          <cell r="C15">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>2016</v>
-          </cell>
-          <cell r="B16">
-            <v>0.76386273888267209</v>
-          </cell>
-          <cell r="C16">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>2017</v>
-          </cell>
-          <cell r="B17">
-            <v>1.0975609756097562</v>
-          </cell>
-          <cell r="C17">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>2018</v>
-          </cell>
-          <cell r="B18">
-            <v>1.5744653015195824</v>
-          </cell>
-          <cell r="C18">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>2019</v>
-          </cell>
-          <cell r="B19">
-            <v>2.2533384110853234</v>
-          </cell>
-          <cell r="C19">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>2020</v>
-          </cell>
-          <cell r="B20">
-            <v>3.2142857142857144</v>
-          </cell>
-          <cell r="C20">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>2021</v>
-          </cell>
-          <cell r="B21">
-            <v>4.5637199338541574</v>
-          </cell>
-          <cell r="C21">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>2022</v>
-          </cell>
-          <cell r="B22">
-            <v>6.4376548985828963</v>
-          </cell>
-          <cell r="C22">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>2023</v>
-          </cell>
-          <cell r="B23">
-            <v>9</v>
-          </cell>
-          <cell r="C23">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>2024</v>
-          </cell>
-          <cell r="B24">
-            <v>12.430507473864703</v>
-          </cell>
-          <cell r="C24">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>2025</v>
-          </cell>
-          <cell r="B25">
-            <v>16.895859910841978</v>
-          </cell>
-          <cell r="C25">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>2026</v>
-          </cell>
-          <cell r="B26">
-            <v>22.5</v>
-          </cell>
-          <cell r="C26">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>2027</v>
-          </cell>
-          <cell r="B27">
-            <v>29.21998399083289</v>
-          </cell>
-          <cell r="C27">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>2028</v>
-          </cell>
-          <cell r="B28">
-            <v>36.851270686751157</v>
-          </cell>
-          <cell r="C28">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>2029</v>
-          </cell>
-          <cell r="B29">
-            <v>45</v>
-          </cell>
-          <cell r="C29">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>2030</v>
-          </cell>
-          <cell r="B30">
-            <v>53.148729313248843</v>
-          </cell>
-          <cell r="C30">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>2031</v>
-          </cell>
-          <cell r="B31">
-            <v>60.780016009167106</v>
-          </cell>
-          <cell r="C31">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>2032</v>
-          </cell>
-          <cell r="B32">
-            <v>67.5</v>
-          </cell>
-          <cell r="C32">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>2033</v>
-          </cell>
-          <cell r="B33">
-            <v>73.104140089158022</v>
-          </cell>
-          <cell r="C33">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>2034</v>
-          </cell>
-          <cell r="B34">
-            <v>77.569492526135292</v>
-          </cell>
-          <cell r="C34">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>2035</v>
-          </cell>
-          <cell r="B35">
-            <v>81</v>
-          </cell>
-          <cell r="C35">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>2036</v>
-          </cell>
-          <cell r="B36">
-            <v>83.562345101417094</v>
-          </cell>
-          <cell r="C36">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>2037</v>
-          </cell>
-          <cell r="B37">
-            <v>85.436280066145841</v>
-          </cell>
-          <cell r="C37">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>2038</v>
-          </cell>
-          <cell r="B38">
-            <v>86.785714285714292</v>
-          </cell>
-          <cell r="C38">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>2039</v>
-          </cell>
-          <cell r="B39">
-            <v>87.746661588914662</v>
-          </cell>
-          <cell r="C39">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>2040</v>
-          </cell>
-          <cell r="B40">
-            <v>88.425534698480405</v>
-          </cell>
-          <cell r="C40">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>2041</v>
-          </cell>
-          <cell r="B41">
-            <v>88.902439024390233</v>
-          </cell>
-          <cell r="C41">
-            <v>90</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1716,57 +1406,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="78.33203125" customWidth="1"/>
+    <col min="1" max="1" width="78.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="56.1" customHeight="1"/>
+    <row r="2" spans="1:1">
       <c r="A2" s="81" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="82" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="83"/>
     </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="30">
       <c r="A5" s="84" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="85"/>
     </row>
-    <row r="7" spans="1:1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="84" customHeight="1">
       <c r="A7" s="84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="84"/>
     </row>
-    <row r="9" spans="1:1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="81.95" customHeight="1">
       <c r="A9" s="86" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="85"/>
     </row>
-    <row r="11" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="78" customHeight="1">
       <c r="A11" s="84" t="s">
         <v>79</v>
       </c>
@@ -1774,7 +1464,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Jp2NPGDxq4ipKSvZio8u5uepMuatkqRKF2qMIacR4bE5gWPmZT21uodFWqY5BWjSr4pWny6SqQj/aPP07qNQwA==" saltValue="0YkILgcRRcpUdMz8SnZf+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1782,37 +1472,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="55.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="3" customWidth="1"/>
-    <col min="6" max="8" width="13.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="3" customWidth="1"/>
+    <col min="6" max="8" width="13.875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="3" customWidth="1"/>
     <col min="10" max="10" width="14" style="3" customWidth="1"/>
-    <col min="11" max="14" width="10.83203125" style="3"/>
-    <col min="15" max="16" width="10.83203125" style="4"/>
-    <col min="17" max="16384" width="10.83203125" style="3"/>
+    <col min="11" max="14" width="10.875" style="3"/>
+    <col min="15" max="16" width="10.875" style="4"/>
+    <col min="17" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="4" customFormat="1">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1830,7 +1520,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="4" customFormat="1">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
         <v>2</v>
@@ -1848,7 +1538,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="4" customFormat="1">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="3"/>
@@ -1864,7 +1554,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="26.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>3</v>
@@ -1882,10 +1572,10 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="6.95" customHeight="1">
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="B7" s="14" t="s">
         <v>67</v>
       </c>
@@ -1908,7 +1598,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15.95" customHeight="1">
       <c r="B8" s="17" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +1621,7 @@
       <c r="O8" s="66"/>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15.95" customHeight="1">
       <c r="B9" s="17" t="s">
         <v>57</v>
       </c>
@@ -1952,7 +1642,7 @@
       <c r="M9" s="66"/>
       <c r="N9" s="66"/>
     </row>
-    <row r="10" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15.95" customHeight="1">
       <c r="B10" s="17" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1664,7 @@
       <c r="M10" s="66"/>
       <c r="N10" s="66"/>
     </row>
-    <row r="11" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15.95" customHeight="1">
       <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +1686,7 @@
       <c r="M11" s="66"/>
       <c r="N11" s="66"/>
     </row>
-    <row r="12" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15.95" customHeight="1">
       <c r="B12" s="17" t="s">
         <v>56</v>
       </c>
@@ -2017,7 +1707,7 @@
       <c r="M12" s="66"/>
       <c r="N12" s="66"/>
     </row>
-    <row r="13" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15.95" customHeight="1">
       <c r="B13" s="17" t="s">
         <v>8</v>
       </c>
@@ -2039,7 +1729,7 @@
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
     </row>
-    <row r="14" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15.95" customHeight="1">
       <c r="B14" s="17" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +1750,7 @@
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="B15" s="17" t="s">
         <v>24</v>
       </c>
@@ -2079,7 +1769,7 @@
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="B16" s="17" t="s">
         <v>14</v>
       </c>
@@ -2103,7 +1793,7 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
@@ -2127,7 +1817,7 @@
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
@@ -2151,7 +1841,7 @@
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="B19" s="17" t="s">
         <v>21</v>
       </c>
@@ -2174,7 +1864,7 @@
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" customHeight="1">
       <c r="B20" s="21" t="s">
         <v>22</v>
       </c>
@@ -2197,7 +1887,7 @@
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="B21" s="21" t="s">
         <v>58</v>
       </c>
@@ -2220,23 +1910,23 @@
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="23">
-        <f>1799.86133487637*0.4</f>
-        <v>719.94453395054802</v>
-      </c>
-      <c r="D22" s="24" t="s">
+    <row r="22" spans="1:14">
+      <c r="B22" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="90">
+        <f>65*52</f>
+        <v>3380</v>
+      </c>
+      <c r="D22" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="E22" s="92" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
@@ -2244,8 +1934,20 @@
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
     </row>
-    <row r="23" spans="1:14" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E23" s="11"/>
+    <row r="23" spans="1:14">
+      <c r="B23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="23">
+        <f>1799.86133487637*0.4</f>
+        <v>719.94453395054802</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="78" t="s">
+        <v>59</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -2256,26 +1958,20 @@
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
     </row>
-    <row r="24" spans="1:14" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="68" t="s">
-        <v>4</v>
-      </c>
+    <row r="24" spans="1:14" ht="8.1" customHeight="1">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" ht="8.1" customHeight="1">
+      <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2286,12 +1982,14 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="29" t="s">
-        <v>26</v>
+    <row r="26" spans="1:14">
+      <c r="C26" s="27" t="s">
+        <v>25</v>
       </c>
       <c r="D26" s="35"/>
-      <c r="E26" s="68"/>
+      <c r="E26" s="68" t="s">
+        <v>4</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2302,15 +2000,12 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="79">
-        <v>0.2591220979029773</v>
+    <row r="27" spans="1:14">
+      <c r="C27" s="29" t="s">
+        <v>26</v>
       </c>
       <c r="D27" s="35"/>
-      <c r="E27" s="28"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -2321,205 +2016,193 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="80">
-        <v>0.72295897177081381</v>
+    <row r="28" spans="1:14">
+      <c r="B28" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="79">
+        <v>0.2591220979029773</v>
       </c>
       <c r="D28" s="35"/>
-      <c r="E28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="32"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="B29" s="74" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="80">
-        <v>3.47</v>
+        <v>0.72295897177081381</v>
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="87" t="s">
+    <row r="30" spans="1:14">
+      <c r="B30" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="80">
+        <v>3.47</v>
+      </c>
+      <c r="D30" s="35"/>
+      <c r="E30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" s="32" customFormat="1">
+      <c r="A31" s="34"/>
+      <c r="B31" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="88">
-        <f>((-C48/(1/(1+C61)+1/((1+C61)^2)+1/((1+C61)^3)+1/((1+C61)^4)+1/((1+C61)^5))+D46)/(1-C54)-D48)/(C10*C13)</f>
-        <v>0.2591220979029773</v>
-      </c>
-      <c r="D30" s="35"/>
-    </row>
-    <row r="31" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="88">
+        <f>((-C50/(1/(1+C63)+1/((1+C63)^2)+1/((1+C63)^3)+1/((1+C63)^4)+1/((1+C63)^5))+D48)/(1-C56)-D50)/(C10*C13)</f>
+        <v>0.28823493166697389</v>
+      </c>
       <c r="D31" s="35"/>
-      <c r="E31" s="8"/>
-      <c r="G31" s="37"/>
-    </row>
-    <row r="32" spans="1:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
+    </row>
+    <row r="32" spans="1:14" s="32" customFormat="1">
+      <c r="A32" s="34"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="8"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="2:16" ht="26.25">
+      <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="34" spans="2:16" ht="20" x14ac:dyDescent="0.25">
-      <c r="B34" s="38" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="35" spans="2:16" ht="19.5">
+      <c r="B35" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" s="39" t="s">
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="40" t="s">
+      <c r="C36" s="13"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="2:16">
+      <c r="B37" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C37" s="41">
         <v>0</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D37" s="41">
         <v>1</v>
       </c>
-      <c r="E36" s="41">
-        <f>D36+1</f>
+      <c r="E37" s="41">
+        <f>D37+1</f>
         <v>2</v>
       </c>
-      <c r="F36" s="41">
-        <f>E36+1</f>
+      <c r="F37" s="41">
+        <f>E37+1</f>
         <v>3</v>
       </c>
-      <c r="G36" s="41">
-        <f>F36+1</f>
+      <c r="G37" s="41">
+        <f>F37+1</f>
         <v>4</v>
       </c>
-      <c r="H36" s="42">
-        <f>G36+1</f>
+      <c r="H37" s="42">
+        <f>G37+1</f>
         <v>5</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="M36" s="43"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="44"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="46"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="47"/>
+      <c r="J37" s="4"/>
       <c r="K37" s="4"/>
+      <c r="M37" s="43"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="31">
-        <f>-SUM(C8:C9)</f>
-        <v>-50000</v>
-      </c>
+    <row r="38" spans="2:16" ht="9" customHeight="1">
+      <c r="B38" s="44"/>
+      <c r="C38" s="45"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="45"/>
       <c r="G38" s="45"/>
       <c r="H38" s="46"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="48"/>
+      <c r="J38" s="47"/>
       <c r="K38" s="4"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:16" ht="17.100000000000001" customHeight="1">
       <c r="B39" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31">
-        <f>-$C$21*$C$13*$C$10</f>
-        <v>-1509.3</v>
-      </c>
-      <c r="E39" s="31">
-        <f>-$C$21*$C$13*$C$10</f>
-        <v>-1509.3</v>
-      </c>
-      <c r="F39" s="31">
-        <f>-$C$21*$C$13*$C$10</f>
-        <v>-1509.3</v>
-      </c>
-      <c r="G39" s="31">
-        <f>-$C$21*$C$13*$C$10</f>
-        <v>-1509.3</v>
-      </c>
-      <c r="H39" s="49">
-        <f>-$C$21*$C$13*$C$10</f>
-        <v>-1509.3</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C39" s="31">
+        <f>-SUM(C8:C9)</f>
+        <v>-50000</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="46"/>
       <c r="I39" s="4"/>
       <c r="J39" s="48"/>
       <c r="K39" s="4"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B40" s="17" t="s">
-        <v>14</v>
+    <row r="40" spans="2:16" ht="17.100000000000001" customHeight="1">
+      <c r="B40" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="31">
-        <f>-$C16*$C$11*$C$13</f>
-        <v>-2323.8226059654635</v>
+        <f>-$C$21*$C$13*$C$10</f>
+        <v>-1509.3</v>
       </c>
       <c r="E40" s="31">
-        <f>-$C16*$C$11*$C$13</f>
-        <v>-2323.8226059654635</v>
+        <f>-$C$21*$C$13*$C$10</f>
+        <v>-1509.3</v>
       </c>
       <c r="F40" s="31">
-        <f>-$C16*$C$11*$C$13</f>
-        <v>-2323.8226059654635</v>
+        <f>-$C$21*$C$13*$C$10</f>
+        <v>-1509.3</v>
       </c>
       <c r="G40" s="31">
-        <f>-$C16*$C$11*$C$13</f>
-        <v>-2323.8226059654635</v>
+        <f>-$C$21*$C$13*$C$10</f>
+        <v>-1509.3</v>
       </c>
       <c r="H40" s="49">
-        <f>-$C16*$C$11*$C$13</f>
-        <v>-2323.8226059654635</v>
+        <f>-$C$21*$C$13*$C$10</f>
+        <v>-1509.3</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="48"/>
@@ -2527,30 +2210,30 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:16">
       <c r="B41" s="17" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="31">
-        <f>-($C17*$C13*$C11)</f>
-        <v>-2944.2096365173288</v>
+        <f>-$C16*$C$11*$C$13</f>
+        <v>-2323.8226059654635</v>
       </c>
       <c r="E41" s="31">
-        <f>-($C17*$C13*$C11)</f>
-        <v>-2944.2096365173288</v>
+        <f>-$C16*$C$11*$C$13</f>
+        <v>-2323.8226059654635</v>
       </c>
       <c r="F41" s="31">
-        <f>-($C17*$C13*$C11)</f>
-        <v>-2944.2096365173288</v>
+        <f>-$C16*$C$11*$C$13</f>
+        <v>-2323.8226059654635</v>
       </c>
       <c r="G41" s="31">
-        <f>-($C17*$C13*$C11)</f>
-        <v>-2944.2096365173288</v>
+        <f>-$C16*$C$11*$C$13</f>
+        <v>-2323.8226059654635</v>
       </c>
       <c r="H41" s="49">
-        <f>-($C17*$C13*$C11)</f>
-        <v>-2944.2096365173288</v>
+        <f>-$C16*$C$11*$C$13</f>
+        <v>-2323.8226059654635</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="48"/>
@@ -2558,30 +2241,30 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:16">
       <c r="B42" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="31">
-        <f>-($C18*$C13*$C11)</f>
-        <v>-2818.1703631153837</v>
+        <f>-($C17*$C13*$C11)</f>
+        <v>-2944.2096365173288</v>
       </c>
       <c r="E42" s="31">
-        <f>-($C18*$C13*$C11)</f>
-        <v>-2818.1703631153837</v>
+        <f>-($C17*$C13*$C11)</f>
+        <v>-2944.2096365173288</v>
       </c>
       <c r="F42" s="31">
-        <f>-($C18*$C13*$C11)</f>
-        <v>-2818.1703631153837</v>
+        <f>-($C17*$C13*$C11)</f>
+        <v>-2944.2096365173288</v>
       </c>
       <c r="G42" s="31">
-        <f>-($C18*$C13*$C11)</f>
-        <v>-2818.1703631153837</v>
+        <f>-($C17*$C13*$C11)</f>
+        <v>-2944.2096365173288</v>
       </c>
       <c r="H42" s="49">
-        <f>-($C18*$C13*$C11)</f>
-        <v>-2818.1703631153837</v>
+        <f>-($C17*$C13*$C11)</f>
+        <v>-2944.2096365173288</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="48"/>
@@ -2589,30 +2272,30 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:16">
       <c r="B43" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="31">
-        <f>-$C19*$C13*$C11</f>
-        <v>-1086.8131868131868</v>
+        <f>-($C18*$C13*$C11)</f>
+        <v>-2818.1703631153837</v>
       </c>
       <c r="E43" s="31">
-        <f>-$C19*$C13*$C11</f>
-        <v>-1086.8131868131868</v>
+        <f>-($C18*$C13*$C11)</f>
+        <v>-2818.1703631153837</v>
       </c>
       <c r="F43" s="31">
-        <f>-$C19*$C13*$C11</f>
-        <v>-1086.8131868131868</v>
+        <f>-($C18*$C13*$C11)</f>
+        <v>-2818.1703631153837</v>
       </c>
       <c r="G43" s="31">
-        <f>-$C19*$C13*$C11</f>
-        <v>-1086.8131868131868</v>
+        <f>-($C18*$C13*$C11)</f>
+        <v>-2818.1703631153837</v>
       </c>
       <c r="H43" s="49">
-        <f>-$C19*$C13*$C11</f>
-        <v>-1086.8131868131868</v>
+        <f>-($C18*$C13*$C11)</f>
+        <v>-2818.1703631153837</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="48"/>
@@ -2620,148 +2303,162 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:16">
       <c r="B44" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="31">
+        <f>-$C19*$C13*$C11</f>
+        <v>-1086.8131868131868</v>
+      </c>
+      <c r="E44" s="31">
+        <f>-$C19*$C13*$C11</f>
+        <v>-1086.8131868131868</v>
+      </c>
+      <c r="F44" s="31">
+        <f>-$C19*$C13*$C11</f>
+        <v>-1086.8131868131868</v>
+      </c>
+      <c r="G44" s="31">
+        <f>-$C19*$C13*$C11</f>
+        <v>-1086.8131868131868</v>
+      </c>
+      <c r="H44" s="49">
+        <f>-$C19*$C13*$C11</f>
+        <v>-1086.8131868131868</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="4"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="2:16">
+      <c r="B45" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31">
         <f>-$C20*$C$10*$C$13</f>
         <v>-4644</v>
       </c>
-      <c r="E44" s="31">
+      <c r="E45" s="31">
         <f>-$C20*$C$10*$C$13</f>
         <v>-4644</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F45" s="31">
         <f>-$C20*$C$10*$C$13</f>
         <v>-4644</v>
       </c>
-      <c r="G44" s="31">
+      <c r="G45" s="31">
         <f>-$C20*$C$10*$C$13</f>
         <v>-4644</v>
       </c>
-      <c r="H44" s="49">
+      <c r="H45" s="49">
         <f>-$C20*$C$10*$C$13</f>
         <v>-4644</v>
       </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="50"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31">
-        <f>-$C$22</f>
-        <v>-719.94453395054802</v>
-      </c>
-      <c r="E45" s="31">
-        <f>-$C$22</f>
-        <v>-719.94453395054802</v>
-      </c>
-      <c r="F45" s="31">
-        <f>-$C$22</f>
-        <v>-719.94453395054802</v>
-      </c>
-      <c r="G45" s="31">
-        <f>-$C$22</f>
-        <v>-719.94453395054802</v>
-      </c>
-      <c r="H45" s="49">
-        <f>-$C$22</f>
-        <v>-719.94453395054802</v>
-      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="48"/>
-      <c r="K45" s="4"/>
+      <c r="K45" s="50"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31">
-        <f>-($C$9+$C$8)/5</f>
-        <v>-10000</v>
-      </c>
-      <c r="E46" s="31">
-        <f t="shared" ref="E46:H46" si="0">-($C$9+$C$8)/5</f>
-        <v>-10000</v>
-      </c>
-      <c r="F46" s="31">
-        <f t="shared" si="0"/>
-        <v>-10000</v>
-      </c>
-      <c r="G46" s="31">
-        <f t="shared" si="0"/>
-        <v>-10000</v>
-      </c>
-      <c r="H46" s="49">
-        <f t="shared" si="0"/>
-        <v>-10000</v>
+    <row r="46" spans="2:16">
+      <c r="B46" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95">
+        <f>-$C$22</f>
+        <v>-3380</v>
+      </c>
+      <c r="E46" s="95">
+        <f>-$C$22</f>
+        <v>-3380</v>
+      </c>
+      <c r="F46" s="95">
+        <f>-$C$22</f>
+        <v>-3380</v>
+      </c>
+      <c r="G46" s="95">
+        <f>-$C$22</f>
+        <v>-3380</v>
+      </c>
+      <c r="H46" s="96">
+        <f>-$C$22</f>
+        <v>-3380</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="48"/>
-      <c r="K46" s="4"/>
+      <c r="K46" s="50"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="17"/>
+    <row r="47" spans="2:16">
+      <c r="B47" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="49"/>
+      <c r="D47" s="31">
+        <f>-$C$23</f>
+        <v>-719.94453395054802</v>
+      </c>
+      <c r="E47" s="31">
+        <f>-$C$23</f>
+        <v>-719.94453395054802</v>
+      </c>
+      <c r="F47" s="31">
+        <f>-$C$23</f>
+        <v>-719.94453395054802</v>
+      </c>
+      <c r="G47" s="31">
+        <f>-$C$23</f>
+        <v>-719.94453395054802</v>
+      </c>
+      <c r="H47" s="49">
+        <f>-$C$23</f>
+        <v>-719.94453395054802</v>
+      </c>
       <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="J47" s="48"/>
       <c r="K47" s="4"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B48" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="52">
-        <f t="shared" ref="C48:H48" si="1">SUM(C38:C46)</f>
-        <v>-50000</v>
-      </c>
-      <c r="D48" s="52">
-        <f>SUM(D38:D46)</f>
-        <v>-26046.260326361909</v>
-      </c>
-      <c r="E48" s="52">
-        <f t="shared" si="1"/>
-        <v>-26046.260326361909</v>
-      </c>
-      <c r="F48" s="52">
-        <f t="shared" si="1"/>
-        <v>-26046.260326361909</v>
-      </c>
-      <c r="G48" s="52">
-        <f t="shared" si="1"/>
-        <v>-26046.260326361909</v>
-      </c>
-      <c r="H48" s="53">
-        <f t="shared" si="1"/>
-        <v>-26046.260326361909</v>
+    <row r="48" spans="2:16">
+      <c r="B48" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31">
+        <f>-($C$9+$C$8)/5</f>
+        <v>-10000</v>
+      </c>
+      <c r="E48" s="31">
+        <f t="shared" ref="E48:H48" si="0">-($C$9+$C$8)/5</f>
+        <v>-10000</v>
+      </c>
+      <c r="F48" s="31">
+        <f t="shared" si="0"/>
+        <v>-10000</v>
+      </c>
+      <c r="G48" s="31">
+        <f t="shared" si="0"/>
+        <v>-10000</v>
+      </c>
+      <c r="H48" s="49">
+        <f t="shared" si="0"/>
+        <v>-10000</v>
       </c>
       <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="J48" s="48"/>
       <c r="K48" s="4"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
     </row>
-    <row r="49" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:16" ht="9" customHeight="1">
       <c r="B49" s="17"/>
       <c r="C49" s="31"/>
       <c r="D49" s="31"/>
@@ -2775,30 +2472,33 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:16">
       <c r="B50" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="52"/>
+        <v>41</v>
+      </c>
+      <c r="C50" s="52">
+        <f t="shared" ref="C50:H50" si="1">SUM(C39:C48)</f>
+        <v>-50000</v>
+      </c>
       <c r="D50" s="52">
-        <f>$C27*$C10*$C13</f>
-        <v>30084.075566535666</v>
+        <f>SUM(D39:D48)</f>
+        <v>-29426.260326361909</v>
       </c>
       <c r="E50" s="52">
-        <f>$C27*$C10*$C13</f>
-        <v>30084.075566535666</v>
+        <f t="shared" si="1"/>
+        <v>-29426.260326361909</v>
       </c>
       <c r="F50" s="52">
-        <f>$C27*$C10*$C13</f>
-        <v>30084.075566535666</v>
+        <f t="shared" si="1"/>
+        <v>-29426.260326361909</v>
       </c>
       <c r="G50" s="52">
-        <f>$C27*$C10*$C13</f>
-        <v>30084.075566535666</v>
+        <f t="shared" si="1"/>
+        <v>-29426.260326361909</v>
       </c>
       <c r="H50" s="53">
-        <f>$C27*$C10*$C13</f>
-        <v>30084.075566535666</v>
+        <f t="shared" si="1"/>
+        <v>-29426.260326361909</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -2806,7 +2506,7 @@
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:16" ht="9" customHeight="1">
       <c r="B51" s="17"/>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
@@ -2820,33 +2520,30 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:16">
       <c r="B52" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="52">
-        <f t="shared" ref="C52:H52" si="2">C48+C50</f>
-        <v>-50000</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C52" s="52"/>
       <c r="D52" s="52">
-        <f t="shared" si="2"/>
-        <v>4037.815240173757</v>
+        <f>$C28*$C10*$C13</f>
+        <v>30084.075566535666</v>
       </c>
       <c r="E52" s="52">
-        <f>E48+E50</f>
-        <v>4037.815240173757</v>
+        <f>$C28*$C10*$C13</f>
+        <v>30084.075566535666</v>
       </c>
       <c r="F52" s="52">
-        <f t="shared" si="2"/>
-        <v>4037.815240173757</v>
+        <f>$C28*$C10*$C13</f>
+        <v>30084.075566535666</v>
       </c>
       <c r="G52" s="52">
-        <f t="shared" si="2"/>
-        <v>4037.815240173757</v>
+        <f>$C28*$C10*$C13</f>
+        <v>30084.075566535666</v>
       </c>
       <c r="H52" s="53">
-        <f t="shared" si="2"/>
-        <v>4037.815240173757</v>
+        <f>$C28*$C10*$C13</f>
+        <v>30084.075566535666</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -2854,12 +2551,10 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
     </row>
-    <row r="53" spans="2:16" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:16" ht="9" customHeight="1">
       <c r="B53" s="17"/>
       <c r="C53" s="31"/>
-      <c r="D53" s="54" t="s">
-        <v>44</v>
-      </c>
+      <c r="D53" s="31"/>
       <c r="E53" s="31"/>
       <c r="F53" s="31"/>
       <c r="G53" s="31"/>
@@ -2870,99 +2565,101 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
     </row>
-    <row r="54" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="56">
-        <v>0.21</v>
+    <row r="54" spans="2:16">
+      <c r="B54" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="52">
+        <f t="shared" ref="C54:H54" si="2">C50+C52</f>
+        <v>-50000</v>
+      </c>
+      <c r="D54" s="52">
+        <f t="shared" si="2"/>
+        <v>657.81524017375705</v>
+      </c>
+      <c r="E54" s="52">
+        <f>E50+E52</f>
+        <v>657.81524017375705</v>
+      </c>
+      <c r="F54" s="52">
+        <f t="shared" si="2"/>
+        <v>657.81524017375705</v>
+      </c>
+      <c r="G54" s="52">
+        <f t="shared" si="2"/>
+        <v>657.81524017375705</v>
+      </c>
+      <c r="H54" s="53">
+        <f t="shared" si="2"/>
+        <v>657.81524017375705</v>
       </c>
       <c r="I54" s="4"/>
-      <c r="J54" s="58"/>
+      <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
     </row>
-    <row r="55" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="77"/>
-      <c r="D55" s="57">
-        <f>-$C$54*D52</f>
-        <v>-847.941200436489</v>
-      </c>
-      <c r="E55" s="57">
-        <f>-$C$54*E52</f>
-        <v>-847.941200436489</v>
-      </c>
-      <c r="F55" s="57">
-        <f>-$C$54*F52</f>
-        <v>-847.941200436489</v>
-      </c>
-      <c r="G55" s="57">
-        <f>-$C$54*G52</f>
-        <v>-847.941200436489</v>
-      </c>
-      <c r="H55" s="72">
-        <f>-$C$54*H52</f>
-        <v>-847.941200436489</v>
-      </c>
+    <row r="55" spans="2:16" ht="12.95" customHeight="1">
+      <c r="B55" s="17"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="49"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="58"/>
+      <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
     </row>
-    <row r="56" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="17"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="49"/>
+    <row r="56" spans="2:16" ht="14.1" customHeight="1">
+      <c r="B56" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="56">
+        <v>0.21</v>
+      </c>
       <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
+      <c r="J56" s="58"/>
       <c r="K56" s="4"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="52">
-        <f>C52</f>
-        <v>-50000</v>
-      </c>
-      <c r="D57" s="52">
-        <f>D52*(1-$C$54)-D46</f>
-        <v>13189.874039737268</v>
-      </c>
-      <c r="E57" s="52">
-        <f t="shared" ref="E57:H57" si="3">E52*(1-$C$54)-E46</f>
-        <v>13189.874039737268</v>
-      </c>
-      <c r="F57" s="52">
-        <f t="shared" si="3"/>
-        <v>13189.874039737268</v>
-      </c>
-      <c r="G57" s="52">
-        <f t="shared" si="3"/>
-        <v>13189.874039737268</v>
-      </c>
-      <c r="H57" s="53">
-        <f t="shared" si="3"/>
-        <v>13189.874039737268</v>
+    <row r="57" spans="2:16" ht="14.1" customHeight="1">
+      <c r="B57" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="77"/>
+      <c r="D57" s="57">
+        <f>-$C$56*D54</f>
+        <v>-138.14120043648899</v>
+      </c>
+      <c r="E57" s="57">
+        <f>-$C$56*E54</f>
+        <v>-138.14120043648899</v>
+      </c>
+      <c r="F57" s="57">
+        <f>-$C$56*F54</f>
+        <v>-138.14120043648899</v>
+      </c>
+      <c r="G57" s="57">
+        <f>-$C$56*G54</f>
+        <v>-138.14120043648899</v>
+      </c>
+      <c r="H57" s="72">
+        <f>-$C$56*H54</f>
+        <v>-138.14120043648899</v>
       </c>
       <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="58"/>
       <c r="K57" s="4"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
     </row>
-    <row r="58" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:16" ht="9" customHeight="1">
       <c r="B58" s="17"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
@@ -2976,33 +2673,33 @@
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:16">
       <c r="B59" s="51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C59" s="52">
-        <f>C57</f>
+        <f>C54</f>
         <v>-50000</v>
       </c>
       <c r="D59" s="52">
-        <f>SUM($C57:D57)</f>
-        <v>-36810.125960262732</v>
+        <f>D54*(1-$C$56)-D48</f>
+        <v>10519.674039737269</v>
       </c>
       <c r="E59" s="52">
-        <f>SUM($C57:E57)</f>
-        <v>-23620.251920525465</v>
+        <f t="shared" ref="E59:H59" si="3">E54*(1-$C$56)-E48</f>
+        <v>10519.674039737269</v>
       </c>
       <c r="F59" s="52">
-        <f>SUM($C57:F57)</f>
-        <v>-10430.377880788197</v>
+        <f t="shared" si="3"/>
+        <v>10519.674039737269</v>
       </c>
       <c r="G59" s="52">
-        <f>SUM($C57:G57)</f>
-        <v>2759.4961589490704</v>
+        <f t="shared" si="3"/>
+        <v>10519.674039737269</v>
       </c>
       <c r="H59" s="53">
-        <f>SUM($C57:H57)</f>
-        <v>15949.370198686338</v>
+        <f t="shared" si="3"/>
+        <v>10519.674039737269</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -3010,39 +2707,55 @@
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:16" ht="9" customHeight="1">
       <c r="B60" s="17"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="19"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="49"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
     </row>
-    <row r="61" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="56">
-        <v>0.1</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="19"/>
+    <row r="61" spans="2:16">
+      <c r="B61" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="52">
+        <f>C59</f>
+        <v>-50000</v>
+      </c>
+      <c r="D61" s="52">
+        <f>SUM($C59:D59)</f>
+        <v>-39480.325960262729</v>
+      </c>
+      <c r="E61" s="52">
+        <f>SUM($C59:E59)</f>
+        <v>-28960.651920525459</v>
+      </c>
+      <c r="F61" s="52">
+        <f>SUM($C59:F59)</f>
+        <v>-18440.977880788188</v>
+      </c>
+      <c r="G61" s="52">
+        <f>SUM($C59:G59)</f>
+        <v>-7921.3038410509198</v>
+      </c>
+      <c r="H61" s="53">
+        <f>SUM($C59:H59)</f>
+        <v>2598.3701986863489</v>
+      </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:16" ht="9" customHeight="1">
       <c r="B62" s="17"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -3056,13 +2769,12 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="59">
-        <f>C57+NPV(C61,D57:H57)</f>
-        <v>0</v>
+    <row r="63" spans="2:16" ht="14.1" customHeight="1">
+      <c r="B63" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="56">
+        <v>0.1</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
@@ -3075,7 +2787,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:16" ht="9" customHeight="1">
       <c r="B64" s="17"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -3083,30 +2795,32 @@
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
       <c r="H64" s="19"/>
+      <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:16">
       <c r="B65" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="60">
-        <f>COUNTIF(C59:H59,"&lt;0")</f>
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="C65" s="59">
+        <f>C59+NPV(C63,D59:H59)</f>
+        <v>-10122.158831674446</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="19"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
     </row>
-    <row r="66" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:16" ht="9" customHeight="1">
       <c r="B66" s="17"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -3119,178 +2833,209 @@
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B67" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="C67" s="62">
-        <f>IRR(C57:H57)</f>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="D67" s="63"/>
-      <c r="E67" s="63"/>
-      <c r="F67" s="63"/>
-      <c r="G67" s="63"/>
-      <c r="H67" s="26"/>
+    <row r="67" spans="2:16">
+      <c r="B67" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="60">
+        <f>COUNTIF(C61:H61,"&lt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="19"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:16" ht="9" customHeight="1">
+      <c r="B68" s="17"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="19"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:16">
+      <c r="B69" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="62">
+        <f>IRR(C59:H59)</f>
+        <v>1.712855680413683E-2</v>
+      </c>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="26"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B70" s="27" t="s">
+    <row r="70" spans="2:16">
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+    </row>
+    <row r="71" spans="2:16">
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+    </row>
+    <row r="72" spans="2:16">
+      <c r="B72" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B71" s="11" t="s">
+    <row r="73" spans="2:16">
+      <c r="B73" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="64"/>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B72" s="11" t="s">
+      <c r="C73" s="64"/>
+    </row>
+    <row r="74" spans="2:16">
+      <c r="B74" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="64"/>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B73" s="11" t="s">
+      <c r="C74" s="65"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="64"/>
+    </row>
+    <row r="75" spans="2:16">
+      <c r="B75" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="C73" s="64"/>
-      <c r="D73" s="64"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B74" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B75" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C75" s="64"/>
       <c r="D75" s="64"/>
       <c r="E75" s="64"/>
       <c r="F75" s="64"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B76" s="4" t="s">
-        <v>72</v>
+    <row r="76" spans="2:16">
+      <c r="B76" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
       <c r="E76" s="64"/>
       <c r="F76" s="64"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:16">
       <c r="B77" s="4" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="C77" s="64"/>
       <c r="D77" s="64"/>
       <c r="E77" s="64"/>
       <c r="F77" s="64"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:16">
       <c r="B78" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C78" s="64"/>
       <c r="D78" s="64"/>
       <c r="E78" s="64"/>
       <c r="F78" s="64"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:16">
+      <c r="B79" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C79" s="64"/>
       <c r="D79" s="64"/>
       <c r="E79" s="64"/>
       <c r="F79" s="64"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="4"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:16">
+      <c r="B80" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+    </row>
+    <row r="83" spans="2:6">
       <c r="B83" s="4"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6">
       <c r="B85" s="4"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6">
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6">
       <c r="B87" s="4"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6">
       <c r="B88" s="4"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6">
       <c r="B89" s="4"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6">
       <c r="B91" s="4"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6">
       <c r="B92" s="4"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6">
       <c r="B93" s="4"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6">
       <c r="B94" s="4"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6">
       <c r="B95" s="4"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6">
       <c r="B96" s="4"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2">
       <c r="B97" s="4"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2">
       <c r="B98" s="4"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2">
       <c r="B99" s="4"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2">
       <c r="B100" s="4"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2">
       <c r="B101" s="4"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="4"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>